<commit_message>
Trying out different cycles for coin cell
</commit_message>
<xml_diff>
--- a/rgbvals.xlsx
+++ b/rgbvals.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="1062">
   <si>
     <t>deeppink 3</t>
   </si>
@@ -3209,22 +3209,7 @@
     <t>V/I=R</t>
   </si>
   <si>
-    <t>18.75V/mA</t>
-  </si>
-  <si>
     <t>ohm=V/A</t>
-  </si>
-  <si>
-    <t>5V</t>
-  </si>
-  <si>
-    <t>4.5V</t>
-  </si>
-  <si>
-    <t>diff from 6V</t>
-  </si>
-  <si>
-    <t>3.7V</t>
   </si>
   <si>
     <t>For 20mA</t>
@@ -26149,10 +26134,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -26160,7 +26145,7 @@
     <col min="10" max="10" width="10.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>1048</v>
       </c>
@@ -26171,10 +26156,10 @@
         <v>1050</v>
       </c>
       <c r="D1" t="s">
-        <v>1065</v>
+        <v>1060</v>
       </c>
       <c r="E1" t="s">
-        <v>1066</v>
+        <v>1061</v>
       </c>
       <c r="G1" t="s">
         <v>1053</v>
@@ -26186,7 +26171,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>16</v>
       </c>
@@ -26214,115 +26199,59 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H4" t="s">
         <v>1057</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H5" t="s">
         <v>1058</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" t="s">
         <v>1051</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H8" t="s">
-        <v>1060</v>
-      </c>
-      <c r="K8" t="s">
-        <v>1061</v>
-      </c>
-      <c r="L8" t="s">
-        <v>1062</v>
-      </c>
-      <c r="M8" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="H9">
-        <f>6/0.32</f>
-        <v>18.75</v>
-      </c>
-      <c r="I9" t="s">
         <v>1059</v>
       </c>
-      <c r="K9">
-        <f>5/G2</f>
-        <v>15.625</v>
-      </c>
-      <c r="L9">
-        <f>4.5/G2</f>
-        <v>14.0625</v>
-      </c>
-      <c r="M9">
-        <f>3.7/G2</f>
-        <v>11.5625</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="J10" t="s">
-        <v>1063</v>
-      </c>
-      <c r="K10">
-        <f>H9-K9</f>
-        <v>3.125</v>
-      </c>
-      <c r="L10">
-        <f>H9-L9</f>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="H11">
+        <f>1.5/G2</f>
         <v>4.6875</v>
       </c>
-      <c r="M10">
-        <f>H9-M9</f>
-        <v>7.1875</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="H12">
+        <f>I14/G2</f>
+        <v>7.1874999999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H13">
-        <f>E2/1000</f>
-        <v>9.5999999999999992E-4</v>
-      </c>
-      <c r="K13" t="s">
-        <v>1061</v>
-      </c>
-      <c r="M13" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="H14">
-        <f>6/H13</f>
-        <v>6250.0000000000009</v>
-      </c>
-      <c r="K14">
-        <f>5/H13</f>
-        <v>5208.3333333333339</v>
-      </c>
-      <c r="M14">
-        <f>3.7/H13</f>
-        <v>3854.166666666667</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="J15" t="s">
-        <v>1063</v>
-      </c>
-      <c r="K15">
-        <f>H14-K14</f>
-        <v>1041.666666666667</v>
-      </c>
-      <c r="M15">
-        <f>H14-M14</f>
-        <v>2395.8333333333339</v>
+        <f>I15/G2</f>
+        <v>7.8125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I14">
+        <f>6-3.7</f>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I15">
+        <f>6-3.5</f>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wipe sequence added to breathe
</commit_message>
<xml_diff>
--- a/rgbvals.xlsx
+++ b/rgbvals.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6888" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6888" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$522</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="1061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="1062">
   <si>
     <t>deeppink 3</t>
   </si>
@@ -3213,6 +3214,9 @@
   </si>
   <si>
     <t>For 60 mA</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -9479,7 +9483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="519" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1039">
+  <cellXfs count="1040">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -12594,6 +12598,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -26258,11 +26265,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -27385,6 +27390,150 @@
       <c r="F124">
         <f t="shared" si="1"/>
         <v>254</v>
+      </c>
+    </row>
+    <row r="125" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E125">
+        <v>126</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="1"/>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="126" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E126">
+        <v>125</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="127" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E127">
+        <v>124</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="1"/>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="128" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E128">
+        <v>123</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="1"/>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="129" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E129">
+        <v>122</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="1"/>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="130" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E130">
+        <v>121</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="1"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="131" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E131">
+        <v>120</v>
+      </c>
+      <c r="F131">
+        <f t="shared" ref="F131:F140" si="2">2*E131</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="132" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E132">
+        <v>119</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="2"/>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="133" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E133">
+        <v>118</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="2"/>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="134" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E134">
+        <v>117</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="2"/>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="135" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E135">
+        <v>116</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="2"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="136" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E136">
+        <v>115</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="2"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="137" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E137">
+        <v>114</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="2"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="138" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E138">
+        <v>113</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="2"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="139" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E139">
+        <v>112</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="2"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="140" spans="5:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E140">
+        <v>111</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="2"/>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -27469,4 +27618,153 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1039">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1039">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1039">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1039">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1039">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1039">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1039">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1039">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1039">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1039">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1039">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1039">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1039">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1039">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1039">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1039">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="J17" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>